<commit_message>
added last update info
</commit_message>
<xml_diff>
--- a/data/list_ex.xlsx
+++ b/data/list_ex.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="691">
   <si>
     <t>ID</t>
   </si>
@@ -1802,6 +1802,9 @@
     <t>Letters, daily calendar, lectures</t>
   </si>
   <si>
+    <t>ediarum.BASE.edit, ediarum.DB, ediarum.WEB</t>
+  </si>
+  <si>
     <t>Arndt</t>
   </si>
   <si>
@@ -2048,6 +2051,73 @@
   </si>
   <si>
     <t>http://suprasliensis.obdurodon.org/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+De filosoof en de filoloog: De correspondentie tussen G. J. P. J. Bolland en P. J. Cosijn (1879-1899)</t>
+  </si>
+  <si>
+    <t>Bolland</t>
+  </si>
+  <si>
+    <t>Gerardus</t>
+  </si>
+  <si>
+    <t>Porck</t>
+  </si>
+  <si>
+    <t>Thijs</t>
+  </si>
+  <si>
+    <t>Leiden University Fund (LUF)</t>
+  </si>
+  <si>
+    <t>Leiden</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>https://www.luf.nl/en</t>
+  </si>
+  <si>
+    <t>"NLD"</t>
+  </si>
+  <si>
+    <t>https://correspondentie-bolland-en-cosijn.huygens.knaw.nl/</t>
+  </si>
+  <si>
+    <t>History of Philosophy</t>
+  </si>
+  <si>
+    <t>ony pdf</t>
+  </si>
+  <si>
+    <t>Ernst Haeckel (1834–1919): Briefedition</t>
+  </si>
+  <si>
+    <t>Haeckel</t>
+  </si>
+  <si>
+    <t>Ernst</t>
+  </si>
+  <si>
+    <t>Bach</t>
+  </si>
+  <si>
+    <t>Friedrich-Schiller-Universität Jena</t>
+  </si>
+  <si>
+    <t>Jena</t>
+  </si>
+  <si>
+    <t>https://www.uni-jena.de/</t>
+  </si>
+  <si>
+    <t>https://haeckel-briefwechsel-projekt.uni-jena.de/de</t>
+  </si>
+  <si>
+    <t>History of Science</t>
   </si>
 </sst>
 </file>
@@ -2386,7 +2456,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AC90"/>
+  <dimension ref="A1:AC93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -8907,6 +8977,9 @@
       <c r="AB77" t="s">
         <v>43</v>
       </c>
+      <c r="AC77" t="s">
+        <v>586</v>
+      </c>
     </row>
     <row r="78" spans="1:29">
       <c r="A78">
@@ -8922,7 +8995,7 @@
         <v>581</v>
       </c>
       <c r="E78" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="F78" t="s">
         <v>454</v>
@@ -8992,6 +9065,9 @@
       </c>
       <c r="AB78" t="s">
         <v>43</v>
+      </c>
+      <c r="AC78" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="79" spans="1:29">
@@ -8999,7 +9075,7 @@
         <v>50</v>
       </c>
       <c r="B79" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C79" t="s">
         <v>580</v>
@@ -9008,7 +9084,7 @@
         <v>581</v>
       </c>
       <c r="E79" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="F79" t="s">
         <v>287</v>
@@ -9078,6 +9154,9 @@
       </c>
       <c r="AB79" t="s">
         <v>43</v>
+      </c>
+      <c r="AC79" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="80" spans="1:29">
@@ -9094,10 +9173,10 @@
         <v>581</v>
       </c>
       <c r="E80" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="F80" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="G80" t="s">
         <v>52</v>
@@ -9171,13 +9250,13 @@
         <v>51</v>
       </c>
       <c r="B81" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="E81" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="G81" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="H81">
         <v>53.3673</v>
@@ -9186,7 +9265,7 @@
         <v>7.2086</v>
       </c>
       <c r="J81" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="K81">
         <v>2930597</v>
@@ -9201,7 +9280,7 @@
         <v>54</v>
       </c>
       <c r="O81" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="P81">
         <v>2021</v>
@@ -9210,13 +9289,13 @@
         <v>111</v>
       </c>
       <c r="R81" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="S81" t="s">
         <v>40</v>
       </c>
       <c r="T81" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="U81" t="s">
         <v>585</v>
@@ -9234,7 +9313,7 @@
         <v>44</v>
       </c>
       <c r="Z81" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="AA81" t="s">
         <v>44</v>
@@ -9251,22 +9330,22 @@
         <v>52</v>
       </c>
       <c r="B82" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="C82" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="D82" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="E82" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="F82" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="G82" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="H82">
         <v>42.8138</v>
@@ -9275,7 +9354,7 @@
         <v>-1.6458</v>
       </c>
       <c r="J82" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="K82">
         <v>3117800</v>
@@ -9287,10 +9366,10 @@
         <v>-1.6458</v>
       </c>
       <c r="N82" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="O82" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="P82">
         <v>2000</v>
@@ -9299,13 +9378,13 @@
         <v>123</v>
       </c>
       <c r="R82" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="S82" t="s">
         <v>125</v>
       </c>
       <c r="T82" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="U82" t="s">
         <v>482</v>
@@ -9337,16 +9416,16 @@
         <v>53</v>
       </c>
       <c r="B83" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E83" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="F83" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="G83" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="H83">
         <v>47.8095</v>
@@ -9370,7 +9449,7 @@
         <v>315</v>
       </c>
       <c r="O83" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="P83">
         <v>2022</v>
@@ -9379,7 +9458,7 @@
         <v>56</v>
       </c>
       <c r="R83" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="S83" t="s">
         <v>125</v>
@@ -9412,7 +9491,7 @@
         <v>43</v>
       </c>
       <c r="AC83" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="84" spans="1:29">
@@ -9420,22 +9499,22 @@
         <v>54</v>
       </c>
       <c r="B84" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="C84" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D84" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="E84" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="F84" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="G84" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="H84">
         <v>51.2562</v>
@@ -9444,7 +9523,7 @@
         <v>7.1508</v>
       </c>
       <c r="J84" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="K84">
         <v>2805753</v>
@@ -9459,7 +9538,7 @@
         <v>54</v>
       </c>
       <c r="O84" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="P84">
         <v>2022</v>
@@ -9468,13 +9547,13 @@
         <v>56</v>
       </c>
       <c r="R84" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="S84" t="s">
         <v>237</v>
       </c>
       <c r="T84" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="U84" t="s">
         <v>74</v>
@@ -9506,22 +9585,22 @@
         <v>54</v>
       </c>
       <c r="B85" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="C85" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D85" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="E85" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="F85" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="G85" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="H85">
         <v>51.2562</v>
@@ -9530,7 +9609,7 @@
         <v>7.1508</v>
       </c>
       <c r="J85" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="K85">
         <v>2805753</v>
@@ -9545,7 +9624,7 @@
         <v>54</v>
       </c>
       <c r="O85" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="P85">
         <v>2022</v>
@@ -9554,13 +9633,13 @@
         <v>56</v>
       </c>
       <c r="R85" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="S85" t="s">
         <v>237</v>
       </c>
       <c r="T85" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="U85" t="s">
         <v>74</v>
@@ -9592,16 +9671,16 @@
         <v>55</v>
       </c>
       <c r="B86" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="C86" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="D86" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="G86" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="H86">
         <v>38.897676</v>
@@ -9610,7 +9689,7 @@
         <v>-77.03653</v>
       </c>
       <c r="J86" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="K86">
         <v>4782977</v>
@@ -9625,7 +9704,7 @@
         <v>121</v>
       </c>
       <c r="O86" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="P86">
         <v>1998</v>
@@ -9634,16 +9713,16 @@
         <v>402</v>
       </c>
       <c r="R86" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="S86" t="s">
         <v>237</v>
       </c>
       <c r="T86" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="U86" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="V86" t="s">
         <v>44</v>
@@ -9672,22 +9751,22 @@
         <v>56</v>
       </c>
       <c r="B87" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="C87" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="D87" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="E87" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="F87" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="G87" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="H87">
         <v>60.3894</v>
@@ -9696,7 +9775,7 @@
         <v>5.3221</v>
       </c>
       <c r="J87" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="K87">
         <v>3161732</v>
@@ -9708,7 +9787,7 @@
         <v>5.3221</v>
       </c>
       <c r="N87" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="O87" t="s">
         <v>417</v>
@@ -9720,16 +9799,16 @@
         <v>56</v>
       </c>
       <c r="R87" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="S87" t="s">
         <v>237</v>
       </c>
       <c r="T87" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="U87" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="V87" t="s">
         <v>43</v>
@@ -9747,7 +9826,7 @@
         <v>45</v>
       </c>
       <c r="AA87" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="AB87" t="s">
         <v>43</v>
@@ -9758,13 +9837,13 @@
         <v>57</v>
       </c>
       <c r="B88" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="C88" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="D88" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="G88" t="s">
         <v>85</v>
@@ -9800,7 +9879,7 @@
         <v>123</v>
       </c>
       <c r="R88" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="S88" t="s">
         <v>125</v>
@@ -9833,7 +9912,7 @@
         <v>43</v>
       </c>
       <c r="AC88" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="89" spans="1:29">
@@ -9841,22 +9920,22 @@
         <v>58</v>
       </c>
       <c r="B89" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="C89" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="D89" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="E89" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="F89" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="G89" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="H89">
         <v>47.3769</v>
@@ -9865,7 +9944,7 @@
         <v>8.5417</v>
       </c>
       <c r="J89" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="K89">
         <v>2657896</v>
@@ -9880,16 +9959,16 @@
         <v>343</v>
       </c>
       <c r="O89" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="P89">
         <v>2011</v>
       </c>
       <c r="Q89" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="R89" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="S89" t="s">
         <v>40</v>
@@ -9898,7 +9977,7 @@
         <v>137</v>
       </c>
       <c r="U89" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="V89" t="s">
         <v>44</v>
@@ -9927,13 +10006,13 @@
         <v>59</v>
       </c>
       <c r="B90" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="E90" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="F90" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="G90" t="s">
         <v>85</v>
@@ -9966,10 +10045,10 @@
         <v>2011</v>
       </c>
       <c r="Q90" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="R90" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="S90" t="s">
         <v>125</v>
@@ -10000,6 +10079,183 @@
       </c>
       <c r="AB90" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="91" spans="1:29">
+      <c r="A91">
+        <v>60</v>
+      </c>
+      <c r="B91" t="s">
+        <v>669</v>
+      </c>
+      <c r="C91" t="s">
+        <v>670</v>
+      </c>
+      <c r="D91" t="s">
+        <v>671</v>
+      </c>
+      <c r="E91" t="s">
+        <v>672</v>
+      </c>
+      <c r="F91" t="s">
+        <v>673</v>
+      </c>
+      <c r="G91" t="s">
+        <v>674</v>
+      </c>
+      <c r="H91">
+        <v>52.160114</v>
+      </c>
+      <c r="I91">
+        <v>4.49701</v>
+      </c>
+      <c r="J91" t="s">
+        <v>675</v>
+      </c>
+      <c r="K91">
+        <v>2751773</v>
+      </c>
+      <c r="L91">
+        <v>52.15833</v>
+      </c>
+      <c r="M91">
+        <v>4.49306</v>
+      </c>
+      <c r="N91" t="s">
+        <v>676</v>
+      </c>
+      <c r="O91" t="s">
+        <v>677</v>
+      </c>
+      <c r="P91">
+        <v>2019</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>678</v>
+      </c>
+      <c r="R91" t="s">
+        <v>679</v>
+      </c>
+      <c r="S91" t="s">
+        <v>40</v>
+      </c>
+      <c r="T91" t="s">
+        <v>680</v>
+      </c>
+      <c r="U91" t="s">
+        <v>565</v>
+      </c>
+      <c r="V91" t="s">
+        <v>43</v>
+      </c>
+      <c r="W91" t="s">
+        <v>43</v>
+      </c>
+      <c r="X91" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y91" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z91" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA91" t="s">
+        <v>681</v>
+      </c>
+      <c r="AB91" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="92" spans="1:29">
+      <c r="A92">
+        <v>61</v>
+      </c>
+      <c r="B92" t="s">
+        <v>682</v>
+      </c>
+      <c r="C92" t="s">
+        <v>683</v>
+      </c>
+      <c r="D92" t="s">
+        <v>684</v>
+      </c>
+      <c r="E92" t="s">
+        <v>685</v>
+      </c>
+      <c r="F92" t="s">
+        <v>445</v>
+      </c>
+      <c r="G92" t="s">
+        <v>686</v>
+      </c>
+      <c r="H92">
+        <v>50.9271</v>
+      </c>
+      <c r="I92">
+        <v>11.5892</v>
+      </c>
+      <c r="J92" t="s">
+        <v>687</v>
+      </c>
+      <c r="K92">
+        <v>2895044</v>
+      </c>
+      <c r="L92">
+        <v>50.92878</v>
+      </c>
+      <c r="M92">
+        <v>11.5899</v>
+      </c>
+      <c r="N92" t="s">
+        <v>54</v>
+      </c>
+      <c r="O92" t="s">
+        <v>688</v>
+      </c>
+      <c r="P92">
+        <v>2017</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>56</v>
+      </c>
+      <c r="R92" t="s">
+        <v>689</v>
+      </c>
+      <c r="S92" t="s">
+        <v>40</v>
+      </c>
+      <c r="T92" t="s">
+        <v>690</v>
+      </c>
+      <c r="U92" t="s">
+        <v>565</v>
+      </c>
+      <c r="V92" t="s">
+        <v>43</v>
+      </c>
+      <c r="W92" t="s">
+        <v>43</v>
+      </c>
+      <c r="X92" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y92" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z92" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA92" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB92" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="93" spans="1:29">
+      <c r="A93">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>